<commit_message>
Adapted chromedriver and its path + Moved driver to its own file
</commit_message>
<xml_diff>
--- a/final_project/user/dashboard.xlsx
+++ b/final_project/user/dashboard.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/2020fa-final-project-DevGlitch/final_project/user/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EDCD2F-4322-7846-A865-D616D917A56E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42111BC-13D4-6447-B760-97AD16297CD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-760" yWindow="880" windowWidth="21900" windowHeight="19580" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
+    <workbookView xWindow="3960" yWindow="760" windowWidth="21900" windowHeight="19580" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
   </bookViews>
   <sheets>
-    <sheet name="dashboard" sheetId="1" r:id="rId1"/>
-    <sheet name="COCO" sheetId="2" r:id="rId2"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="comments" sheetId="4" r:id="rId2"/>
+    <sheet name="coco" sheetId="2" r:id="rId3"/>
+    <sheet name="emojis" sheetId="5" r:id="rId4"/>
+    <sheet name="Draft" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
-  <si>
-    <t>TAGS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="189">
   <si>
     <t>OBJECT</t>
   </si>
@@ -292,12 +292,6 @@
     <t>* Only one target object can be selected</t>
   </si>
   <si>
-    <t>* You can have up to 10 targetted tags and/or accounts</t>
-  </si>
-  <si>
-    <t>* All of these can be changed anytime prior running the bot</t>
-  </si>
-  <si>
     <t>kingcharlescavalier</t>
   </si>
   <si>
@@ -358,17 +352,257 @@
     <t>object</t>
   </si>
   <si>
-    <t>tags</t>
-  </si>
-  <si>
     <t>accounts</t>
+  </si>
+  <si>
+    <t>Awwww</t>
+  </si>
+  <si>
+    <t>Wow! In love!! 😍😍</t>
+  </si>
+  <si>
+    <t>Sooooo cute!!</t>
+  </si>
+  <si>
+    <t>Cute!</t>
+  </si>
+  <si>
+    <t>Lovely dog you got there!</t>
+  </si>
+  <si>
+    <t>OMG this is so cute!!</t>
+  </si>
+  <si>
+    <t>Beautiful picture</t>
+  </si>
+  <si>
+    <t>Awww so cute!! How old is your dog?</t>
+  </si>
+  <si>
+    <t>Love this pic of your dog, look so cute!!</t>
+  </si>
+  <si>
+    <t>The cutest pic I've seen today</t>
+  </si>
+  <si>
+    <t>Awww your dog just stole my heart</t>
+  </si>
+  <si>
+    <t>I think we need to call heaven as they obviously lost an angel!</t>
+  </si>
+  <si>
+    <t>Gorgeous!</t>
+  </si>
+  <si>
+    <t>Beautiful!</t>
+  </si>
+  <si>
+    <t>Wonderful!</t>
+  </si>
+  <si>
+    <t>Amazing!</t>
+  </si>
+  <si>
+    <t>Too cute!!</t>
+  </si>
+  <si>
+    <t>Looking gorgeous</t>
+  </si>
+  <si>
+    <t>Too perfect</t>
+  </si>
+  <si>
+    <t>So pretty</t>
+  </si>
+  <si>
+    <t>Perfection</t>
+  </si>
+  <si>
+    <t>Perfection at its best</t>
+  </si>
+  <si>
+    <t>This picture made my day</t>
+  </si>
+  <si>
+    <t>Too much beauty</t>
+  </si>
+  <si>
+    <t>Cuteness overload!</t>
+  </si>
+  <si>
+    <t>Did your dog swallow magnets? Cause he is so attractive! Lol</t>
+  </si>
+  <si>
+    <t>Is your dog name WiFi? Because I'm really feeling a connection haha</t>
+  </si>
+  <si>
+    <t>Your dog is so cute its distracting</t>
+  </si>
+  <si>
+    <t>Does your dog has a name or can I call him Mine? Haha</t>
+  </si>
+  <si>
+    <t>10/10 for this cuteness</t>
+  </si>
+  <si>
+    <t>😍</t>
+  </si>
+  <si>
+    <t>🤣</t>
+  </si>
+  <si>
+    <t>😂</t>
+  </si>
+  <si>
+    <t>😁</t>
+  </si>
+  <si>
+    <t>🥰</t>
+  </si>
+  <si>
+    <t>🤩</t>
+  </si>
+  <si>
+    <t>😜</t>
+  </si>
+  <si>
+    <t>😄</t>
+  </si>
+  <si>
+    <t>😆</t>
+  </si>
+  <si>
+    <t>😅</t>
+  </si>
+  <si>
+    <t>😱</t>
+  </si>
+  <si>
+    <t>❤️</t>
+  </si>
+  <si>
+    <t>👍</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMG!! Such a hot dog!! Hahaha </t>
+  </si>
+  <si>
+    <t>🐶</t>
+  </si>
+  <si>
+    <t>🐕</t>
+  </si>
+  <si>
+    <t>🐾</t>
+  </si>
+  <si>
+    <t>🌹</t>
+  </si>
+  <si>
+    <t>🌺</t>
+  </si>
+  <si>
+    <t>🌭</t>
+  </si>
+  <si>
+    <t>Look at that sweet face</t>
+  </si>
+  <si>
+    <t>Oh my, so cute!</t>
+  </si>
+  <si>
+    <t>Oh my so gorgeous</t>
+  </si>
+  <si>
+    <t>Your dog is so beautiful!!</t>
+  </si>
+  <si>
+    <t>Little beauty</t>
+  </si>
+  <si>
+    <t>So adorable</t>
+  </si>
+  <si>
+    <t>Omg this is so precious</t>
+  </si>
+  <si>
+    <t>Cutie</t>
+  </si>
+  <si>
+    <t>Adorable!!</t>
+  </si>
+  <si>
+    <t>Such an angel!</t>
+  </si>
+  <si>
+    <t>Lil cutie!!</t>
+  </si>
+  <si>
+    <t>Hello goregous!</t>
+  </si>
+  <si>
+    <t>Awww you are adorable</t>
+  </si>
+  <si>
+    <t>Wow, what a look</t>
+  </si>
+  <si>
+    <t>Omg</t>
+  </si>
+  <si>
+    <t>Such a sweatheart</t>
+  </si>
+  <si>
+    <t>Lovely picture</t>
+  </si>
+  <si>
+    <t>Awww so sweet</t>
+  </si>
+  <si>
+    <t>The cutest dog</t>
+  </si>
+  <si>
+    <t>This is so adorable and pawfect!!</t>
+  </si>
+  <si>
+    <t>Pawfect!</t>
+  </si>
+  <si>
+    <t>Awww adorable!</t>
+  </si>
+  <si>
+    <t>Ridiculously adorable</t>
+  </si>
+  <si>
+    <t>That sweet face</t>
+  </si>
+  <si>
+    <t>hashtags</t>
+  </si>
+  <si>
+    <t>HASHTAGS</t>
+  </si>
+  <si>
+    <t>* You can have up to 10 targetted hashtags and/or accounts</t>
+  </si>
+  <si>
+    <t>* All of these can be changed anytime prior to running the bot</t>
+  </si>
+  <si>
+    <t>ENTER A LIST OF COMMENT HERE. TRY TO HAVE THEM RELATED TO YOUR TARGET OBJECT. A MINIMUM OF 50 COMMENTS IS RECOMMENDED. ALSO IF YOU WOULD LIKE TO ADD EMOJIS PLEASE CHECK THE TAB EMOJIS FOR THE ONES YOU CAN USE.</t>
+  </si>
+  <si>
+    <t>* Make sure to enter a list of comments (see tab comments)</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -426,6 +660,20 @@
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.79998168889431442"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -550,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -620,14 +868,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -952,7 +1215,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -971,32 +1234,32 @@
     <col min="12" max="16384" width="10.83203125" style="12" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>111</v>
+    <row r="1" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="A2" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
     </row>
     <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D3" s="9"/>
@@ -1018,7 +1281,7 @@
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -1043,7 +1306,7 @@
     <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="14"/>
       <c r="C7" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -1056,7 +1319,7 @@
     <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
-        <v>88</v>
+        <v>184</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1069,7 +1332,7 @@
     <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>89</v>
+        <v>187</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1081,7 +1344,9 @@
     </row>
     <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B10" s="14"/>
-      <c r="C10" s="16"/>
+      <c r="C10" s="14" t="s">
+        <v>185</v>
+      </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -1096,17 +1361,17 @@
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="B12" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
     </row>
     <row r="13" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="17"/>
@@ -1123,15 +1388,15 @@
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="22" t="s">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -1140,16 +1405,12 @@
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
     </row>
@@ -1158,13 +1419,9 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
     </row>
@@ -1173,13 +1430,9 @@
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="F17" s="2"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="3" t="s">
-        <v>101</v>
-      </c>
+      <c r="H17" s="3"/>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
     </row>
@@ -1188,13 +1441,9 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="3" t="s">
-        <v>102</v>
-      </c>
+      <c r="H18" s="3"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
     </row>
@@ -1203,13 +1452,9 @@
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="H19" s="3"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
     </row>
@@ -1218,13 +1463,9 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="H20" s="3"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
     </row>
@@ -1233,13 +1474,9 @@
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
-      <c r="F21" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="17"/>
-      <c r="H21" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="H21" s="3"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
     </row>
@@ -1248,28 +1485,20 @@
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="17"/>
-      <c r="H22" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="H22" s="3"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="2:10" ht="20" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
-      <c r="F23" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="17"/>
-      <c r="H23" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="H23" s="4"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
     </row>
@@ -1278,13 +1507,9 @@
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="F24" s="5"/>
       <c r="G24" s="17"/>
-      <c r="H24" s="6" t="s">
-        <v>107</v>
-      </c>
+      <c r="H24" s="6"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
     </row>
@@ -1326,7 +1551,7 @@
       <c r="F29" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <sortState ref="F15:F24">
     <sortCondition ref="F15:F24"/>
   </sortState>
@@ -1340,7 +1565,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select your target object" xr:uid="{FCAA8740-D868-EF42-881C-98502D1E6242}">
           <x14:formula1>
-            <xm:f>COCO!$A$1:$A$80</xm:f>
+            <xm:f>coco!$A$1:$A$80</xm:f>
           </x14:formula1>
           <xm:sqref>D15</xm:sqref>
         </x14:dataValidation>
@@ -1351,6 +1576,318 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FED1C54-6127-4B4B-9967-A134B40B186C}">
+  <dimension ref="A1:XFC62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="96.1640625" style="32" customWidth="1"/>
+    <col min="2" max="16382" width="10.83203125" style="32" hidden="1"/>
+    <col min="16383" max="16383" width="10.83203125" style="32" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="14" style="32" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="31" customFormat="1" ht="88" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00275071-6DCA-514F-8FC5-74605328D697}">
   <dimension ref="A1:A81"/>
   <sheetViews>
@@ -1364,402 +1901,402 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" hidden="1" x14ac:dyDescent="0.2"/>
@@ -1770,4 +2307,473 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7403E4-4282-3947-AFC7-2DFE4F66DE1D}">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="37" zeroHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="29" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="30" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" s="29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" s="29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A6" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A8" s="29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A9" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A10" s="29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A11" s="29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A12" s="29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A13" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A14" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCCE3AF-5D6D-E14B-971C-020231627BC8}">
+  <dimension ref="C3:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="20" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G13" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G19" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G20" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G21" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G23" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G24" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G25" s="32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G26" s="32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G29" s="32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G31" s="32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G32" s="32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G36" s="32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G40" s="32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G41" s="32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="32" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="32" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G46" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="32" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G48" s="32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G50" s="32" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G51" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G52" s="32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G53" s="32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G54" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G55" s="32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G56" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G57" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Switched to Firefox due to Chrome no support of unitest > FFFF
</commit_message>
<xml_diff>
--- a/final_project/user/dashboard.xlsx
+++ b/final_project/user/dashboard.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/2020fa-final-project-DevGlitch/final_project/user/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42111BC-13D4-6447-B760-97AD16297CD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246C2EE7-E1A3-0C43-8A6A-962006A1E87F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="760" windowWidth="21900" windowHeight="19580" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
+    <workbookView xWindow="3960" yWindow="720" windowWidth="21900" windowHeight="19580" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="comments" sheetId="4" r:id="rId2"/>
     <sheet name="coco" sheetId="2" r:id="rId3"/>
-    <sheet name="emojis" sheetId="5" r:id="rId4"/>
-    <sheet name="Draft" sheetId="3" r:id="rId5"/>
+    <sheet name="emoj" sheetId="5" r:id="rId4"/>
+    <sheet name="emojis" sheetId="6" r:id="rId5"/>
+    <sheet name="Draft" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="190">
   <si>
     <t>OBJECT</t>
   </si>
@@ -596,6 +597,9 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>motorcycle</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1219,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1408,7 +1412,9 @@
         <v>17</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="G15" s="17"/>
       <c r="H15" s="3"/>
       <c r="I15" s="17"/>
@@ -2314,7 +2320,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="37" zeroHeight="1" x14ac:dyDescent="0.45"/>
@@ -2419,12 +2425,26 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1436F58-168E-3A4A-9BFA-1EA521BF828A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCCE3AF-5D6D-E14B-971C-020231627BC8}">
   <dimension ref="C3:G57"/>
   <sheetViews>

</xml_diff>

<commit_message>
Implemented new functions to shorten cli code
</commit_message>
<xml_diff>
--- a/final_project/user/dashboard.xlsx
+++ b/final_project/user/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/2020fa-final-project-DevGlitch/final_project/user/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A13B2D4-C546-334A-851B-31D8D822E626}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE10767-86EC-5048-A60D-519FB60B5206}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3960" yWindow="720" windowWidth="21900" windowHeight="19580" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
   </bookViews>
@@ -18,9 +18,6 @@
     <sheet name="coco" sheetId="2" r:id="rId3"/>
     <sheet name="emojis" sheetId="5" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="171">
   <si>
     <t>OBJECT</t>
   </si>
@@ -282,9 +279,6 @@
     <t>DASHBOARD</t>
   </si>
   <si>
-    <t>cavalier</t>
-  </si>
-  <si>
     <t>ACCOUNTS</t>
   </si>
   <si>
@@ -543,10 +537,10 @@
     <t>Awww so sweet 🐾😍</t>
   </si>
   <si>
-    <t>cavaliernationig</t>
-  </si>
-  <si>
     <t>ENTER A LIST OF COMMENT HERE. TRY TO HAVE THEM RELATED TO YOUR TARGET OBJECT. A MINIMUM OF 50 COMMENTS IS RECOMMENDED. ALSO IF YOU WOULD LIKE TO ADD EMOJIS PLEASE CHECK THE TAB EMOJIS FOR A SAMPLE OF THE ONES YOU CAN USE.</t>
+  </si>
+  <si>
+    <t>tapisdeselle</t>
   </si>
 </sst>
 </file>
@@ -838,13 +832,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -867,19 +861,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Draft"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1182,7 +1163,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1203,30 +1184,30 @@
   <sheetData>
     <row r="1" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D1" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1" s="28"/>
       <c r="F1" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="7" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D3" s="9"/>
@@ -1248,7 +1229,7 @@
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -1273,7 +1254,7 @@
     <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B7" s="14"/>
       <c r="C7" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -1286,7 +1267,7 @@
     <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1299,7 +1280,7 @@
     <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1312,7 +1293,7 @@
     <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -1328,17 +1309,17 @@
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
     </row>
     <row r="13" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="17"/>
@@ -1359,11 +1340,11 @@
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="17"/>
@@ -1376,12 +1357,10 @@
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="2" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="3" t="s">
-        <v>170</v>
-      </c>
+      <c r="H15" s="3"/>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
     </row>
@@ -1390,9 +1369,7 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="17"/>
       <c r="H16" s="3"/>
       <c r="I16" s="17"/>
@@ -1566,287 +1543,287 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="31" customFormat="1" ht="88" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
@@ -2301,102 +2278,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="37" t="s">
-        <v>125</v>
+      <c r="A19" s="35" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated functions + added new ones to target accounts
</commit_message>
<xml_diff>
--- a/final_project/user/dashboard.xlsx
+++ b/final_project/user/dashboard.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/2020fa-final-project-DevGlitch/final_project/user/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Documents/GitHub/botwizer/final_project/user/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE10767-86EC-5048-A60D-519FB60B5206}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D305B4-C0CD-4D45-BDAF-F674AAA4B51C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="720" windowWidth="21900" windowHeight="19580" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="25620" windowHeight="20620" activeTab="1" xr2:uid="{3D8CD276-3A0A-4040-8725-AD25C6EA8337}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>OBJECT</t>
   </si>
@@ -294,9 +294,6 @@
     <t>accounts</t>
   </si>
   <si>
-    <t>Sooooo cute!!</t>
-  </si>
-  <si>
     <t>😍</t>
   </si>
   <si>
@@ -372,175 +369,10 @@
     <t>comments</t>
   </si>
   <si>
-    <t>Awwww 😍😍</t>
-  </si>
-  <si>
-    <t>Wow! In love!! 😍❤️❤️</t>
-  </si>
-  <si>
-    <t>Lovely dog you got there! 🐾</t>
-  </si>
-  <si>
-    <t>Cute! 🐾</t>
-  </si>
-  <si>
-    <t>Beautiful picture 🐶 👍</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Awww so cute!! 🤩 How old is your dog? </t>
-  </si>
-  <si>
-    <t>OMG this is so cute!! 🤩🤩</t>
-  </si>
-  <si>
-    <t>Love this pic of your dog, look so cute!! 🥰</t>
-  </si>
-  <si>
-    <t>Awww your dog just stole my heart ❤️</t>
-  </si>
-  <si>
-    <t>The cutest pic I've seen today! 😍</t>
-  </si>
-  <si>
     <t>😇</t>
   </si>
   <si>
-    <t>I think we need to call heaven as they obviously lost an angel! 😇😁😜</t>
-  </si>
-  <si>
-    <t>Gorgeous! 🌹</t>
-  </si>
-  <si>
-    <t>Amazing! 🤩</t>
-  </si>
-  <si>
-    <t>Beautiful! 🌺</t>
-  </si>
-  <si>
-    <t>Wonderful! 🐾</t>
-  </si>
-  <si>
-    <t>Looking gorgeous 😍😍🌹</t>
-  </si>
-  <si>
-    <t>Too cute!! 🥰🥰🥰</t>
-  </si>
-  <si>
-    <t>Too perfect 🤩🤩</t>
-  </si>
-  <si>
-    <t>Perfection 🐶</t>
-  </si>
-  <si>
-    <t>So pretty 🐶🐶</t>
-  </si>
-  <si>
-    <t>Perfection at its best 🐾 😍</t>
-  </si>
-  <si>
-    <t>This picture made my day 😁❤️</t>
-  </si>
-  <si>
-    <t>Too much beauty 🌹🌹🌹</t>
-  </si>
-  <si>
-    <t>Cuteness overload! 😱❤️</t>
-  </si>
-  <si>
-    <t>Did your dog swallow magnets? Cause he is so attractive! 🤣🤣❤️</t>
-  </si>
-  <si>
-    <t>Does your dog has a name or can I call him Mine? Haha 🤣🤣😜</t>
-  </si>
-  <si>
-    <t>Is your dog name WiFi? Because I'm really feeling a connection haha 😜😁</t>
-  </si>
-  <si>
-    <t>Your dog is so cute its distracting 😄😍</t>
-  </si>
-  <si>
-    <t>10/10 for this cuteness 🌹</t>
-  </si>
-  <si>
-    <t>OMG!! Such a hot dog 🌭!! Hahaha  🤣🤣🤣</t>
-  </si>
-  <si>
-    <t>Look at that sweet face 😍😍</t>
-  </si>
-  <si>
-    <t>Oh my, so cute! 🥰🥰🥰</t>
-  </si>
-  <si>
-    <t>Little beauty 👍❤️❤️❤️</t>
-  </si>
-  <si>
-    <t>Your dog is so beautiful!! ❤️❤️❤️</t>
-  </si>
-  <si>
-    <t>Hello goregous! 😁🌹</t>
-  </si>
-  <si>
-    <t>Awww you are adorable 🤩🤩</t>
-  </si>
-  <si>
-    <t>Wow, what a look 👍👍👍</t>
-  </si>
-  <si>
-    <t>Omg 😱❤️❤️❤️</t>
-  </si>
-  <si>
-    <t>Such a sweatheart 😍😍😍</t>
-  </si>
-  <si>
-    <t>Lovely picture 🐾🥰</t>
-  </si>
-  <si>
-    <t>The cutest dog 🌺🐾</t>
-  </si>
-  <si>
-    <t>This is so adorable and pawfect!! 🐾🐾</t>
-  </si>
-  <si>
-    <t>Pawfect! 🐾🐾🐾</t>
-  </si>
-  <si>
-    <t>Ridiculously adorable 😱😍😍</t>
-  </si>
-  <si>
-    <t>That sweet face 🐶😍</t>
-  </si>
-  <si>
-    <t>Awww adorable! 🐶🥰🥰</t>
-  </si>
-  <si>
-    <t>Such an angel! 😇😇</t>
-  </si>
-  <si>
-    <t>Adorable!! 🤩🤩</t>
-  </si>
-  <si>
-    <t>Cutie 😍😍</t>
-  </si>
-  <si>
-    <t>Omg this is so precious 😱🐾❤️</t>
-  </si>
-  <si>
-    <t>So adorable 👍👍👍</t>
-  </si>
-  <si>
-    <t>Lil cutie!! 👍❤️</t>
-  </si>
-  <si>
-    <t>Oh my so gorgeous ❤️</t>
-  </si>
-  <si>
-    <t>Awww so sweet 🐾😍</t>
-  </si>
-  <si>
     <t>ENTER A LIST OF COMMENT HERE. TRY TO HAVE THEM RELATED TO YOUR TARGET OBJECT. A MINIMUM OF 50 COMMENTS IS RECOMMENDED. ALSO IF YOU WOULD LIKE TO ADD EMOJIS PLEASE CHECK THE TAB EMOJIS FOR A SAMPLE OF THE ONES YOU CAN USE.</t>
-  </si>
-  <si>
-    <t>tapisdeselle</t>
   </si>
 </sst>
 </file>
@@ -1162,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDC6BD97-53FD-DD45-B7B7-AAB1362859CE}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1173,9 +1005,9 @@
     <col min="3" max="3" width="3.83203125" style="12" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="3.83203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" style="7" customWidth="1"/>
     <col min="7" max="7" width="3.83203125" style="12" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="30.1640625" style="12" customWidth="1"/>
     <col min="9" max="9" width="3.83203125" style="12" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" style="12" customWidth="1"/>
     <col min="11" max="11" width="12" style="8" customWidth="1"/>
@@ -1188,7 +1020,7 @@
       </c>
       <c r="E1" s="28"/>
       <c r="F1" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>87</v>
@@ -1267,7 +1099,7 @@
     <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1280,7 +1112,7 @@
     <row r="9" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1293,7 +1125,7 @@
     <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -1340,7 +1172,7 @@
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="23" t="s">
@@ -1352,13 +1184,9 @@
     <row r="15" spans="1:11" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="2" t="s">
-        <v>170</v>
-      </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="17"/>
       <c r="H15" s="3"/>
       <c r="I15" s="17"/>
@@ -1501,7 +1329,7 @@
       <c r="F29" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ee8XUWmknwO9FnWyW7UBwZTBNHTKcW9z9JE4xWRX/+WI6UL+LG50D4kXi3cFpg1VDqWp4w2N7eE6QP2h0e+wzA==" saltValue="hJ1y6+RuK4MqvyhIT/RP5g==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tt1YVpW96KVcw2KjibCJuCcrR+wPUh+Bd2G0+ZcvLyoHEHJrSO83TP5N3gonzNEA3K7f9QhKfj5WHyiCbCsXoQ==" saltValue="oMWMjQc5TZunAgo0jHmgIQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <sortState ref="F15:F24">
     <sortCondition ref="F15:F24"/>
   </sortState>
@@ -1529,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FED1C54-6127-4B4B-9967-A134B40B186C}">
   <dimension ref="A1:XFC62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1543,294 +1371,74 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:1" s="31" customFormat="1" ht="88" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="32" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="32" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="32" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="32" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="32" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="32" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="32" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="17" x14ac:dyDescent="0.2"/>
+    <row r="18" x14ac:dyDescent="0.2"/>
+    <row r="19" x14ac:dyDescent="0.2"/>
+    <row r="20" x14ac:dyDescent="0.2"/>
+    <row r="21" x14ac:dyDescent="0.2"/>
+    <row r="22" x14ac:dyDescent="0.2"/>
+    <row r="23" x14ac:dyDescent="0.2"/>
+    <row r="24" x14ac:dyDescent="0.2"/>
+    <row r="25" x14ac:dyDescent="0.2"/>
+    <row r="26" x14ac:dyDescent="0.2"/>
+    <row r="27" x14ac:dyDescent="0.2"/>
+    <row r="28" x14ac:dyDescent="0.2"/>
+    <row r="29" x14ac:dyDescent="0.2"/>
+    <row r="30" x14ac:dyDescent="0.2"/>
+    <row r="31" x14ac:dyDescent="0.2"/>
+    <row r="32" x14ac:dyDescent="0.2"/>
+    <row r="33" x14ac:dyDescent="0.2"/>
+    <row r="34" x14ac:dyDescent="0.2"/>
+    <row r="35" x14ac:dyDescent="0.2"/>
+    <row r="36" x14ac:dyDescent="0.2"/>
+    <row r="37" x14ac:dyDescent="0.2"/>
+    <row r="38" x14ac:dyDescent="0.2"/>
+    <row r="39" x14ac:dyDescent="0.2"/>
+    <row r="40" x14ac:dyDescent="0.2"/>
+    <row r="41" x14ac:dyDescent="0.2"/>
+    <row r="42" x14ac:dyDescent="0.2"/>
+    <row r="43" x14ac:dyDescent="0.2"/>
+    <row r="44" x14ac:dyDescent="0.2"/>
+    <row r="45" x14ac:dyDescent="0.2"/>
+    <row r="46" x14ac:dyDescent="0.2"/>
+    <row r="47" x14ac:dyDescent="0.2"/>
+    <row r="48" x14ac:dyDescent="0.2"/>
+    <row r="49" x14ac:dyDescent="0.2"/>
+    <row r="50" x14ac:dyDescent="0.2"/>
+    <row r="51" x14ac:dyDescent="0.2"/>
+    <row r="52" x14ac:dyDescent="0.2"/>
+    <row r="53" x14ac:dyDescent="0.2"/>
+    <row r="54" x14ac:dyDescent="0.2"/>
+    <row r="55" x14ac:dyDescent="0.2"/>
+    <row r="56" x14ac:dyDescent="0.2"/>
+    <row r="57" x14ac:dyDescent="0.2"/>
+    <row r="58" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="59" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="60" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="61" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="62" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="T+JQcl7feGZFJEPuG3OeH7xJ4u1n+aw/w9GwoA2u0kRO9Hn687AnHhzT21Yqa+KVq2IFnSWpea6xvNilFvclkQ==" saltValue="T+fZIilLwOJwqkgZl0pZng==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState ref="A3:A57">
@@ -2278,102 +1886,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="35" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>